<commit_message>
Change to creating a hierarchal structure for the tool
Instead of using numbers, the xsl now uses the subseries reference and
association id to create a recursion through all the referenced
subseries and files
</commit_message>
<xml_diff>
--- a/example_collection.xlsx
+++ b/example_collection.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Special\ArchivesSpace_authority_project\XEAT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\XEAT\XEAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Template" sheetId="2" r:id="rId2"/>
     <sheet name="Example" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="87">
   <si>
     <t>title</t>
   </si>
@@ -221,6 +221,72 @@
   </si>
   <si>
     <t>Please read the instructions packaged with this spreadsheet before proceeding</t>
+  </si>
+  <si>
+    <t>Series I.</t>
+  </si>
+  <si>
+    <t>Subseries I.A.</t>
+  </si>
+  <si>
+    <t>Subseries II.A.</t>
+  </si>
+  <si>
+    <t>subseries_reference</t>
+  </si>
+  <si>
+    <t>files_reference</t>
+  </si>
+  <si>
+    <t>Files I.A.</t>
+  </si>
+  <si>
+    <t>Subseries II.B.</t>
+  </si>
+  <si>
+    <t>Files II.A.</t>
+  </si>
+  <si>
+    <t>Files II.B.</t>
+  </si>
+  <si>
+    <t>Subseries II.B.I.</t>
+  </si>
+  <si>
+    <t>Files II.B.I.</t>
+  </si>
+  <si>
+    <t>Subseries II.B.II.</t>
+  </si>
+  <si>
+    <t>Files II.B.II.</t>
+  </si>
+  <si>
+    <t>Subseries II.A.,Subseries II.B.</t>
+  </si>
+  <si>
+    <t>Subseries II.B.I. , Subseries II.B.II.</t>
+  </si>
+  <si>
+    <t>Subseries Two A Title</t>
+  </si>
+  <si>
+    <t>Subseries Two B ONE</t>
+  </si>
+  <si>
+    <t>Subseries Two B TWO</t>
+  </si>
+  <si>
+    <t>File Two B Title</t>
+  </si>
+  <si>
+    <t>File One B Title</t>
+  </si>
+  <si>
+    <t>File Two A Title</t>
+  </si>
+  <si>
+    <t>File One A Title</t>
   </si>
 </sst>
 </file>
@@ -255,7 +321,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -274,6 +340,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -287,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -298,6 +400,39 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -599,44 +734,44 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
@@ -645,13 +780,13 @@
       <c r="M4" s="6"/>
     </row>
     <row r="5" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
@@ -660,13 +795,13 @@
       <c r="M5" s="6"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -675,13 +810,13 @@
       <c r="M6" s="6"/>
     </row>
     <row r="7" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -1450,10 +1585,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AC1"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S33" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,86 +1618,92 @@
     <col min="27" max="27" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>54</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1573,607 +1714,891 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA18"/>
+  <dimension ref="A1:AC20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>54</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" t="str">
+      <c r="D2" t="str">
         <f>LOWER("series")</f>
         <v>series</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="O2" s="5"/>
+      <c r="E2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="8"/>
       <c r="Q2" s="5"/>
-      <c r="T2" t="s">
+      <c r="S2" s="5"/>
+      <c r="V2" t="s">
         <v>52</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>45</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>46</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
         <v>47</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>48</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AB2" t="s">
         <v>50</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>36</v>
       </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-      <c r="O3" s="5"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="12" t="s">
+        <v>70</v>
+      </c>
       <c r="Q3" s="5"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="S3" s="5"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
         <v>31</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>35</v>
       </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="I4">
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="K4">
         <v>2000</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>42</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>59</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>60</v>
-      </c>
-      <c r="O4" s="5">
-        <v>1</v>
-      </c>
-      <c r="P4" t="s">
-        <v>61</v>
       </c>
       <c r="Q4" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="R4" t="s">
+        <v>61</v>
+      </c>
+      <c r="S4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
         <v>31</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>35</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="I5">
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="K5">
         <v>2000</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>42</v>
       </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>59</v>
       </c>
-      <c r="N5" t="s">
+      <c r="P5" t="s">
         <v>60</v>
-      </c>
-      <c r="O5" s="5">
-        <v>1</v>
-      </c>
-      <c r="P5" t="s">
-        <v>61</v>
       </c>
       <c r="Q5" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="R5" t="s">
+        <v>61</v>
+      </c>
+      <c r="S5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>35</v>
       </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="K6" t="s">
         <v>40</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>42</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>59</v>
       </c>
-      <c r="N6" t="s">
+      <c r="P6" t="s">
         <v>60</v>
       </c>
-      <c r="O6" s="5">
+      <c r="Q6" s="5">
         <v>1</v>
       </c>
-      <c r="P6" t="s">
+      <c r="R6" t="s">
         <v>61</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="S6" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>34</v>
       </c>
-      <c r="D7">
+      <c r="E7" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="Q7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="V7" t="s">
+        <v>52</v>
+      </c>
+      <c r="W7" t="s">
+        <v>45</v>
+      </c>
+      <c r="X7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="V8" t="s">
+        <v>52</v>
+      </c>
+      <c r="W8" t="s">
+        <v>45</v>
+      </c>
+      <c r="X8" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" t="s">
+        <v>53</v>
+      </c>
+      <c r="K9">
+        <v>2004</v>
+      </c>
+      <c r="L9" t="s">
+        <v>42</v>
+      </c>
+      <c r="O9" t="s">
+        <v>62</v>
+      </c>
+      <c r="P9" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q9" s="5">
         <v>2</v>
       </c>
-      <c r="O7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="T7" t="s">
+      <c r="S9" s="5"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="K10">
+        <v>2005</v>
+      </c>
+      <c r="L10" t="s">
+        <v>42</v>
+      </c>
+      <c r="O10" t="s">
+        <v>62</v>
+      </c>
+      <c r="P10" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>2</v>
+      </c>
+      <c r="S10" s="5"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="V11" t="s">
         <v>52</v>
       </c>
-      <c r="U7" t="s">
+      <c r="W11" t="s">
         <v>45</v>
       </c>
-      <c r="V7" t="s">
+      <c r="X11" t="s">
         <v>46</v>
       </c>
-      <c r="W7" t="s">
+      <c r="Y11" t="s">
         <v>47</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Z11" t="s">
         <v>48</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="AA11" t="s">
         <v>49</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AB11" t="s">
         <v>50</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AC11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="K12" t="s">
+        <v>41</v>
+      </c>
+      <c r="L12" t="s">
+        <v>43</v>
+      </c>
+      <c r="O12" t="s">
+        <v>59</v>
+      </c>
+      <c r="P12" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>3</v>
+      </c>
+      <c r="S12" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="K13">
+        <v>2005</v>
+      </c>
+      <c r="L13" t="s">
+        <v>42</v>
+      </c>
+      <c r="O13" t="s">
+        <v>59</v>
+      </c>
+      <c r="P13" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>3</v>
+      </c>
+      <c r="S13" s="5">
+        <v>2</v>
+      </c>
+      <c r="V13" t="s">
+        <v>52</v>
+      </c>
+      <c r="W13" t="s">
+        <v>45</v>
+      </c>
+      <c r="X13" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" t="s">
         <v>36</v>
       </c>
-      <c r="D8">
-        <v>20</v>
-      </c>
-      <c r="O8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="T8" t="s">
+      <c r="E14" s="8"/>
+      <c r="F14" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="V14" t="s">
         <v>52</v>
       </c>
-      <c r="U8" t="s">
+      <c r="W14" t="s">
         <v>45</v>
       </c>
-      <c r="V8" t="s">
+      <c r="X14" t="s">
         <v>46</v>
       </c>
-      <c r="W8" t="s">
+      <c r="Y14" t="s">
         <v>47</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Z14" t="s">
         <v>48</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="AA14" t="s">
         <v>49</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AB14" t="s">
         <v>50</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AC14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" t="s">
         <v>35</v>
       </c>
-      <c r="D9">
-        <v>20</v>
-      </c>
-      <c r="F9">
-        <v>5</v>
-      </c>
-      <c r="G9" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" t="s">
-        <v>53</v>
-      </c>
-      <c r="I9">
-        <v>2004</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="K15" t="s">
+        <v>41</v>
+      </c>
+      <c r="L15" t="s">
+        <v>43</v>
+      </c>
+      <c r="O15" t="s">
+        <v>59</v>
+      </c>
+      <c r="P15" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>3</v>
+      </c>
+      <c r="S15" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="K16">
+        <v>2005</v>
+      </c>
+      <c r="L16" t="s">
         <v>42</v>
       </c>
-      <c r="M9" t="s">
-        <v>62</v>
-      </c>
-      <c r="N9" t="s">
-        <v>63</v>
-      </c>
-      <c r="O9" s="5">
+      <c r="O16" t="s">
+        <v>59</v>
+      </c>
+      <c r="P16" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q16" s="5">
+        <v>3</v>
+      </c>
+      <c r="S16" s="5">
         <v>2</v>
       </c>
-      <c r="Q9" s="5"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="V16" t="s">
+        <v>52</v>
+      </c>
+      <c r="W16" t="s">
+        <v>45</v>
+      </c>
+      <c r="X16" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="V17" t="s">
+        <v>52</v>
+      </c>
+      <c r="W17" t="s">
+        <v>45</v>
+      </c>
+      <c r="X17" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" t="s">
         <v>35</v>
       </c>
-      <c r="D10">
-        <v>20</v>
-      </c>
-      <c r="I10">
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="K18" t="s">
+        <v>41</v>
+      </c>
+      <c r="L18" t="s">
+        <v>43</v>
+      </c>
+      <c r="O18" t="s">
+        <v>59</v>
+      </c>
+      <c r="P18" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q18" s="5">
+        <v>3</v>
+      </c>
+      <c r="S18" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A19" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="K19">
         <v>2005</v>
       </c>
-      <c r="J10" t="s">
+      <c r="L19" t="s">
         <v>42</v>
       </c>
-      <c r="M10" t="s">
-        <v>62</v>
-      </c>
-      <c r="N10" t="s">
-        <v>63</v>
-      </c>
-      <c r="O10" s="5">
+      <c r="O19" t="s">
+        <v>59</v>
+      </c>
+      <c r="P19" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q19" s="5">
+        <v>3</v>
+      </c>
+      <c r="S19" s="5">
         <v>2</v>
       </c>
-      <c r="Q10" s="5"/>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11">
-        <v>21</v>
-      </c>
-      <c r="O11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="T11" t="s">
+      <c r="V19" t="s">
         <v>52</v>
       </c>
-      <c r="U11" t="s">
+      <c r="W19" t="s">
         <v>45</v>
       </c>
-      <c r="V11" t="s">
+      <c r="X19" t="s">
         <v>46</v>
       </c>
-      <c r="W11" t="s">
+      <c r="Y19" t="s">
         <v>47</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Z19" t="s">
         <v>48</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="AA19" t="s">
         <v>49</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="AB19" t="s">
         <v>50</v>
       </c>
-      <c r="AA11" t="s">
+      <c r="AC19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12">
-        <v>21</v>
-      </c>
-      <c r="I12" t="s">
-        <v>41</v>
-      </c>
-      <c r="J12" t="s">
-        <v>43</v>
-      </c>
-      <c r="M12" t="s">
-        <v>59</v>
-      </c>
-      <c r="N12" t="s">
-        <v>55</v>
-      </c>
-      <c r="O12" s="5">
-        <v>3</v>
-      </c>
-      <c r="Q12" s="5">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="I13">
+      <c r="I20" t="s">
+        <v>58</v>
+      </c>
+      <c r="J20" t="s">
+        <v>38</v>
+      </c>
+      <c r="K20" t="s">
+        <v>39</v>
+      </c>
+      <c r="L20" t="s">
+        <v>42</v>
+      </c>
+      <c r="M20">
+        <v>2000</v>
+      </c>
+      <c r="N20">
         <v>2005</v>
       </c>
-      <c r="J13" t="s">
-        <v>42</v>
-      </c>
-      <c r="M13" t="s">
-        <v>59</v>
-      </c>
-      <c r="N13" t="s">
-        <v>55</v>
-      </c>
-      <c r="O13" s="5">
-        <v>3</v>
-      </c>
-      <c r="Q13" s="5">
-        <v>2</v>
-      </c>
-      <c r="T13" t="s">
+      <c r="Q20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="V20" t="s">
         <v>52</v>
       </c>
-      <c r="U13" t="s">
+      <c r="W20" t="s">
         <v>45</v>
       </c>
-      <c r="V13" t="s">
+      <c r="X20" t="s">
         <v>46</v>
       </c>
-      <c r="W13" t="s">
+      <c r="Y20" t="s">
         <v>47</v>
       </c>
-      <c r="X13" t="s">
+      <c r="Z20" t="s">
         <v>48</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="AA20" t="s">
         <v>49</v>
       </c>
-      <c r="Z13" t="s">
+      <c r="AB20" t="s">
         <v>50</v>
       </c>
-      <c r="AA13" t="s">
+      <c r="AC20" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14" t="s">
-        <v>58</v>
-      </c>
-      <c r="H14" t="s">
-        <v>38</v>
-      </c>
-      <c r="I14" t="s">
-        <v>39</v>
-      </c>
-      <c r="J14" t="s">
-        <v>42</v>
-      </c>
-      <c r="K14">
-        <v>2000</v>
-      </c>
-      <c r="L14">
-        <v>2005</v>
-      </c>
-      <c r="O14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="T14" t="s">
-        <v>52</v>
-      </c>
-      <c r="U14" t="s">
-        <v>45</v>
-      </c>
-      <c r="V14" t="s">
-        <v>46</v>
-      </c>
-      <c r="W14" t="s">
-        <v>47</v>
-      </c>
-      <c r="X14" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="O15" s="5"/>
-      <c r="Q15" s="5"/>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="O16" s="5"/>
-      <c r="Q16" s="5"/>
-    </row>
-    <row r="17" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O17" s="5"/>
-      <c r="Q17" s="5"/>
-    </row>
-    <row r="18" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O18" s="5"/>
-      <c r="Q18" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Instructions for paragraph creation
</commit_message>
<xml_diff>
--- a/example_collection.xlsx
+++ b/example_collection.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="87">
   <si>
     <t>title</t>
   </si>
@@ -1585,10 +1585,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC1"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,6 +1707,11 @@
         <v>24</v>
       </c>
     </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1716,8 +1721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add General Notes and Files able to reference files
</commit_message>
<xml_diff>
--- a/example_collection.xlsx
+++ b/example_collection.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="3" r:id="rId1"/>
     <sheet name="Template" sheetId="2" r:id="rId2"/>
     <sheet name="Example" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" calcMode="manual"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="91">
   <si>
     <t>title</t>
   </si>
@@ -118,12 +118,6 @@
     <t>Subseries Two Title</t>
   </si>
   <si>
-    <t>File Two Title</t>
-  </si>
-  <si>
-    <t>File One Title</t>
-  </si>
-  <si>
     <t>Guide to the Collection title</t>
   </si>
   <si>
@@ -280,13 +274,31 @@
     <t>File Two B Title</t>
   </si>
   <si>
-    <t>File One B Title</t>
-  </si>
-  <si>
     <t>File Two A Title</t>
   </si>
   <si>
     <t>File One A Title</t>
+  </si>
+  <si>
+    <t>generalnote</t>
+  </si>
+  <si>
+    <t>File inside File</t>
+  </si>
+  <si>
+    <t>test general</t>
+  </si>
+  <si>
+    <t>File Two B Two Title</t>
+  </si>
+  <si>
+    <t>File One B Two Title</t>
+  </si>
+  <si>
+    <t>File One B One Title</t>
+  </si>
+  <si>
+    <t>File Two B Two One</t>
   </si>
 </sst>
 </file>
@@ -297,7 +309,7 @@
     <numFmt numFmtId="164" formatCode="00000"/>
     <numFmt numFmtId="165" formatCode="00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,8 +332,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -376,6 +395,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -389,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -421,9 +446,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -444,6 +466,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -727,51 +762,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="A1" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+      <c r="A4" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
@@ -780,13 +815,13 @@
       <c r="M4" s="6"/>
     </row>
     <row r="5" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
@@ -795,13 +830,13 @@
       <c r="M5" s="6"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -810,13 +845,13 @@
       <c r="M6" s="6"/>
     </row>
     <row r="7" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -1585,10 +1620,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="R55" sqref="R55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1616,9 +1651,10 @@
     <col min="25" max="25" width="8" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="10" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1632,10 +1668,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
@@ -1674,13 +1710,13 @@
         <v>15</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="T1" t="s">
         <v>16</v>
       </c>
       <c r="U1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="V1" t="s">
         <v>17</v>
@@ -1706,30 +1742,32 @@
       <c r="AC1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="E2" t="s">
-        <v>66</v>
-      </c>
+      <c r="AD1" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="E2" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC20"/>
+  <dimension ref="A1:AD21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.140625" customWidth="1"/>
@@ -1755,9 +1793,10 @@
     <col min="27" max="27" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1771,10 +1810,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
@@ -1813,13 +1852,13 @@
         <v>15</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="T1" t="s">
         <v>16</v>
       </c>
       <c r="U1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="V1" t="s">
         <v>17</v>
@@ -1845,10 +1884,13 @@
       <c r="AC1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD1" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
@@ -1857,63 +1899,66 @@
         <f>LOWER("series")</f>
         <v>series</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>66</v>
+      <c r="E2" s="25" t="s">
+        <v>64</v>
       </c>
       <c r="F2" s="8"/>
       <c r="Q2" s="5"/>
       <c r="S2" s="5"/>
       <c r="V2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="W2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y2" t="s">
         <v>45</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>46</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>47</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AB2" t="s">
         <v>48</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
         <v>49</v>
       </c>
-      <c r="AB2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Q3" s="5"/>
       <c r="S3" s="5"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
@@ -1921,33 +1966,33 @@
         <v>2000</v>
       </c>
       <c r="L4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="P4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q4" s="5">
         <v>1</v>
       </c>
       <c r="R4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S4" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
@@ -1955,149 +2000,149 @@
         <v>2000</v>
       </c>
       <c r="L5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="P5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q5" s="5">
         <v>1</v>
       </c>
       <c r="R5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S5" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="K6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" t="s">
         <v>40</v>
       </c>
-      <c r="L6" t="s">
-        <v>42</v>
-      </c>
       <c r="O6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="P6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q6" s="5">
         <v>1</v>
       </c>
       <c r="R6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S6" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
         <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F7" s="8"/>
       <c r="Q7" s="5"/>
       <c r="S7" s="5"/>
       <c r="V7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="W7" t="s">
+        <v>43</v>
+      </c>
+      <c r="X7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y7" t="s">
         <v>45</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Z7" t="s">
         <v>46</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="AA7" t="s">
         <v>47</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AB7" t="s">
         <v>48</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AC7" t="s">
         <v>49</v>
       </c>
-      <c r="AB7" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q8" s="5"/>
       <c r="S8" s="5"/>
       <c r="V8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="W8" t="s">
+        <v>43</v>
+      </c>
+      <c r="X8" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y8" t="s">
         <v>45</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Z8" t="s">
         <v>46</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="AA8" t="s">
         <v>47</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AB8" t="s">
         <v>48</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AC8" t="s">
         <v>49</v>
       </c>
-      <c r="AB8" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
@@ -2105,37 +2150,37 @@
         <v>5</v>
       </c>
       <c r="I9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K9">
         <v>2004</v>
       </c>
       <c r="L9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="P9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Q9" s="5">
         <v>2</v>
       </c>
       <c r="S9" s="5"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
@@ -2143,85 +2188,85 @@
         <v>2005</v>
       </c>
       <c r="L10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="P10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Q10" s="5">
         <v>2</v>
       </c>
       <c r="S10" s="5"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>79</v>
+        <v>34</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>77</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Q11" s="5"/>
       <c r="S11" s="5"/>
       <c r="V11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="W11" t="s">
+        <v>43</v>
+      </c>
+      <c r="X11" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y11" t="s">
         <v>45</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Z11" t="s">
         <v>46</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="AA11" t="s">
         <v>47</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="AB11" t="s">
         <v>48</v>
       </c>
-      <c r="AA11" t="s">
+      <c r="AC11" t="s">
         <v>49</v>
       </c>
-      <c r="AB11" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="K12" t="s">
+        <v>39</v>
+      </c>
+      <c r="L12" t="s">
         <v>41</v>
       </c>
-      <c r="L12" t="s">
-        <v>43</v>
-      </c>
       <c r="O12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="P12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q12" s="5">
         <v>3</v>
@@ -2230,15 +2275,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -2246,13 +2291,13 @@
         <v>2005</v>
       </c>
       <c r="L13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="P13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q13" s="5">
         <v>3</v>
@@ -2261,94 +2306,94 @@
         <v>2</v>
       </c>
       <c r="V13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="W13" t="s">
+        <v>43</v>
+      </c>
+      <c r="X13" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y13" t="s">
         <v>45</v>
       </c>
-      <c r="X13" t="s">
+      <c r="Z13" t="s">
         <v>46</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="AA13" t="s">
         <v>47</v>
       </c>
-      <c r="Z13" t="s">
+      <c r="AB13" t="s">
         <v>48</v>
       </c>
-      <c r="AA13" t="s">
+      <c r="AC13" t="s">
         <v>49</v>
       </c>
-      <c r="AB13" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E14" s="8"/>
-      <c r="F14" s="19" t="s">
-        <v>75</v>
+      <c r="F14" s="18" t="s">
+        <v>73</v>
       </c>
       <c r="Q14" s="5"/>
       <c r="S14" s="5"/>
       <c r="V14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="W14" t="s">
+        <v>43</v>
+      </c>
+      <c r="X14" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y14" t="s">
         <v>45</v>
       </c>
-      <c r="X14" t="s">
+      <c r="Z14" t="s">
         <v>46</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="AA14" t="s">
         <v>47</v>
       </c>
-      <c r="Z14" t="s">
+      <c r="AB14" t="s">
         <v>48</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="AC14" t="s">
         <v>49</v>
       </c>
-      <c r="AB14" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
-        <v>75</v>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="K15" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" t="s">
         <v>41</v>
       </c>
-      <c r="L15" t="s">
-        <v>43</v>
-      </c>
       <c r="O15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="P15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q15" s="5">
         <v>3</v>
@@ -2357,15 +2402,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>75</v>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -2373,13 +2418,13 @@
         <v>2005</v>
       </c>
       <c r="L16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="P16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q16" s="5">
         <v>3</v>
@@ -2388,94 +2433,94 @@
         <v>2</v>
       </c>
       <c r="V16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="W16" t="s">
+        <v>43</v>
+      </c>
+      <c r="X16" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y16" t="s">
         <v>45</v>
       </c>
-      <c r="X16" t="s">
+      <c r="Z16" t="s">
         <v>46</v>
       </c>
-      <c r="Y16" t="s">
+      <c r="AA16" t="s">
         <v>47</v>
       </c>
-      <c r="Z16" t="s">
+      <c r="AB16" t="s">
         <v>48</v>
       </c>
-      <c r="AA16" t="s">
+      <c r="AC16" t="s">
         <v>49</v>
       </c>
-      <c r="AB16" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E17" s="8"/>
-      <c r="F17" s="20" t="s">
-        <v>77</v>
+      <c r="F17" s="19" t="s">
+        <v>75</v>
       </c>
       <c r="Q17" s="5"/>
       <c r="S17" s="5"/>
       <c r="V17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="W17" t="s">
+        <v>43</v>
+      </c>
+      <c r="X17" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y17" t="s">
         <v>45</v>
       </c>
-      <c r="X17" t="s">
+      <c r="Z17" t="s">
         <v>46</v>
       </c>
-      <c r="Y17" t="s">
+      <c r="AA17" t="s">
         <v>47</v>
       </c>
-      <c r="Z17" t="s">
+      <c r="AB17" t="s">
         <v>48</v>
       </c>
-      <c r="AA17" t="s">
+      <c r="AC17" t="s">
         <v>49</v>
       </c>
-      <c r="AB17" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
-        <v>77</v>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>75</v>
       </c>
       <c r="B18" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="K18" t="s">
+        <v>39</v>
+      </c>
+      <c r="L18" t="s">
         <v>41</v>
       </c>
-      <c r="L18" t="s">
-        <v>43</v>
-      </c>
       <c r="O18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="P18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q18" s="5">
         <v>3</v>
@@ -2484,29 +2529,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>77</v>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>75</v>
       </c>
       <c r="B19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="D19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
       <c r="K19">
         <v>2005</v>
       </c>
       <c r="L19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="P19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q19" s="5">
         <v>3</v>
@@ -2515,91 +2562,149 @@
         <v>2</v>
       </c>
       <c r="V19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="W19" t="s">
+        <v>43</v>
+      </c>
+      <c r="X19" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y19" t="s">
         <v>45</v>
       </c>
-      <c r="X19" t="s">
+      <c r="Z19" t="s">
         <v>46</v>
       </c>
-      <c r="Y19" t="s">
+      <c r="AA19" t="s">
         <v>47</v>
       </c>
-      <c r="Z19" t="s">
+      <c r="AB19" t="s">
         <v>48</v>
       </c>
-      <c r="AA19" t="s">
+      <c r="AC19" t="s">
         <v>49</v>
       </c>
-      <c r="AB19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="s">
+        <v>85</v>
+      </c>
       <c r="B20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="D20" t="s">
         <v>33</v>
       </c>
       <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" t="s">
+      <c r="F20" s="27"/>
+      <c r="K20">
+        <v>2005</v>
+      </c>
+      <c r="L20" t="s">
+        <v>40</v>
+      </c>
+      <c r="O20" t="s">
+        <v>57</v>
+      </c>
+      <c r="P20" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q20" s="5">
+        <v>3</v>
+      </c>
+      <c r="S20" s="5">
+        <v>2</v>
+      </c>
+      <c r="V20" t="s">
+        <v>50</v>
+      </c>
+      <c r="W20" t="s">
+        <v>43</v>
+      </c>
+      <c r="X20" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>56</v>
+      </c>
+      <c r="J21" t="s">
+        <v>36</v>
+      </c>
+      <c r="K21" t="s">
         <v>37</v>
       </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="I20" t="s">
-        <v>58</v>
-      </c>
-      <c r="J20" t="s">
-        <v>38</v>
-      </c>
-      <c r="K20" t="s">
-        <v>39</v>
-      </c>
-      <c r="L20" t="s">
-        <v>42</v>
-      </c>
-      <c r="M20">
+      <c r="L21" t="s">
+        <v>40</v>
+      </c>
+      <c r="M21">
         <v>2000</v>
       </c>
-      <c r="N20">
+      <c r="N21">
         <v>2005</v>
       </c>
-      <c r="Q20" s="5"/>
-      <c r="S20" s="5"/>
-      <c r="V20" t="s">
-        <v>52</v>
-      </c>
-      <c r="W20" t="s">
+      <c r="Q21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="V21" t="s">
+        <v>50</v>
+      </c>
+      <c r="W21" t="s">
+        <v>43</v>
+      </c>
+      <c r="X21" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y21" t="s">
         <v>45</v>
       </c>
-      <c r="X20" t="s">
+      <c r="Z21" t="s">
         <v>46</v>
       </c>
-      <c r="Y20" t="s">
+      <c r="AA21" t="s">
         <v>47</v>
       </c>
-      <c r="Z20" t="s">
+      <c r="AB21" t="s">
         <v>48</v>
       </c>
-      <c r="AA20" t="s">
+      <c r="AC21" t="s">
         <v>49</v>
       </c>
-      <c r="AB20" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC20" t="s">
-        <v>51</v>
+      <c r="AD21" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Allow files to be at top level entity when missing association_id
</commit_message>
<xml_diff>
--- a/example_collection.xlsx
+++ b/example_collection.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="93">
   <si>
     <t>title</t>
   </si>
@@ -299,6 +299,12 @@
   </si>
   <si>
     <t>File Two B Two One</t>
+  </si>
+  <si>
+    <t>Top level file</t>
+  </si>
+  <si>
+    <t>Top level file with files</t>
   </si>
 </sst>
 </file>
@@ -455,18 +461,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -479,6 +473,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -762,51 +768,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
@@ -815,13 +821,13 @@
       <c r="M4" s="6"/>
     </row>
     <row r="5" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
@@ -830,13 +836,13 @@
       <c r="M5" s="6"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -845,13 +851,13 @@
       <c r="M6" s="6"/>
     </row>
     <row r="7" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -1622,7 +1628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="R55" sqref="R55"/>
     </sheetView>
   </sheetViews>
@@ -1747,7 +1753,7 @@
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="E2" s="24"/>
+      <c r="E2" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1757,16 +1763,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD21"/>
+  <dimension ref="A1:AD23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
@@ -1899,7 +1905,7 @@
         <f>LOWER("series")</f>
         <v>series</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="21" t="s">
         <v>64</v>
       </c>
       <c r="F2" s="8"/>
@@ -2540,7 +2546,7 @@
         <v>33</v>
       </c>
       <c r="E19" s="8"/>
-      <c r="F19" s="26" t="s">
+      <c r="F19" s="22" t="s">
         <v>85</v>
       </c>
       <c r="K19">
@@ -2587,7 +2593,7 @@
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="22" t="s">
         <v>85</v>
       </c>
       <c r="B20" t="s">
@@ -2597,7 +2603,7 @@
         <v>33</v>
       </c>
       <c r="E20" s="8"/>
-      <c r="F20" s="27"/>
+      <c r="F20" s="23"/>
       <c r="K20">
         <v>2005</v>
       </c>
@@ -2642,68 +2648,153 @@
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A21" s="23"/>
       <c r="B21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" t="s">
-        <v>35</v>
-      </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="I21" t="s">
-        <v>56</v>
-      </c>
-      <c r="J21" t="s">
-        <v>36</v>
-      </c>
-      <c r="K21" t="s">
-        <v>37</v>
+      <c r="F21" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="K21">
+        <v>2005</v>
       </c>
       <c r="L21" t="s">
         <v>40</v>
       </c>
-      <c r="M21">
-        <v>2000</v>
-      </c>
-      <c r="N21">
-        <v>2005</v>
-      </c>
-      <c r="Q21" s="5"/>
-      <c r="S21" s="5"/>
+      <c r="O21" t="s">
+        <v>57</v>
+      </c>
+      <c r="P21" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q21" s="5">
+        <v>3</v>
+      </c>
+      <c r="S21" s="5">
+        <v>2</v>
+      </c>
       <c r="V21" t="s">
         <v>50</v>
       </c>
-      <c r="W21" t="s">
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A22" s="23"/>
+      <c r="B22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="23"/>
+      <c r="K22">
+        <v>2005</v>
+      </c>
+      <c r="L22" t="s">
+        <v>40</v>
+      </c>
+      <c r="O22" t="s">
+        <v>57</v>
+      </c>
+      <c r="P22" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q22" s="5">
+        <v>3</v>
+      </c>
+      <c r="S22" s="5">
+        <v>2</v>
+      </c>
+      <c r="V22" t="s">
+        <v>50</v>
+      </c>
+      <c r="W22" t="s">
         <v>43</v>
       </c>
-      <c r="X21" t="s">
+      <c r="X22" t="s">
         <v>44</v>
       </c>
-      <c r="Y21" t="s">
+      <c r="Y22" t="s">
         <v>45</v>
       </c>
-      <c r="Z21" t="s">
+      <c r="Z22" t="s">
         <v>46</v>
       </c>
-      <c r="AA21" t="s">
+      <c r="AA22" t="s">
         <v>47</v>
       </c>
-      <c r="AB21" t="s">
+      <c r="AB22" t="s">
         <v>48</v>
       </c>
-      <c r="AC21" t="s">
+      <c r="AC22" t="s">
         <v>49</v>
       </c>
-      <c r="AD21" t="s">
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>56</v>
+      </c>
+      <c r="J23" t="s">
+        <v>36</v>
+      </c>
+      <c r="K23" t="s">
+        <v>37</v>
+      </c>
+      <c r="L23" t="s">
+        <v>40</v>
+      </c>
+      <c r="M23">
+        <v>2000</v>
+      </c>
+      <c r="N23">
+        <v>2005</v>
+      </c>
+      <c r="Q23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="V23" t="s">
+        <v>50</v>
+      </c>
+      <c r="W23" t="s">
+        <v>43</v>
+      </c>
+      <c r="X23" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD23" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add customizable Access Note and User Restriction Notes
</commit_message>
<xml_diff>
--- a/example_collection.xlsx
+++ b/example_collection.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\XEAT\XEAT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\XACT\XACT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="98">
   <si>
     <t>title</t>
   </si>
@@ -305,6 +305,21 @@
   </si>
   <si>
     <t>Top level file with files</t>
+  </si>
+  <si>
+    <t>accessrestrict</t>
+  </si>
+  <si>
+    <t>userestrict</t>
+  </si>
+  <si>
+    <t>TEST ACCESS</t>
+  </si>
+  <si>
+    <t>TEST Restrict</t>
+  </si>
+  <si>
+    <t>File One A Title &amp; two</t>
   </si>
 </sst>
 </file>
@@ -1626,10 +1641,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R55" sqref="R55"/>
+      <selection activeCell="AE35" sqref="AE35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1658,9 +1673,10 @@
     <col min="26" max="26" width="10" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1751,8 +1767,14 @@
       <c r="AD1" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="E2" s="20"/>
     </row>
   </sheetData>
@@ -1763,10 +1785,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD23"/>
+  <dimension ref="A1:AF23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S28" sqref="S28"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1799,10 +1821,12 @@
     <col min="27" max="27" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="23.140625" customWidth="1"/>
+    <col min="32" max="32" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1893,8 +1917,14 @@
       <c r="AD1" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -1938,8 +1968,14 @@
       <c r="AD2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>64</v>
       </c>
@@ -1956,12 +1992,12 @@
       <c r="Q3" s="5"/>
       <c r="S3" s="5"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="D4" t="s">
         <v>33</v>
@@ -1990,7 +2026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>68</v>
       </c>
@@ -2024,7 +2060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>68</v>
       </c>
@@ -2057,8 +2093,11 @@
       <c r="S6" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AF6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>63</v>
       </c>
@@ -2099,7 +2138,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>65</v>
       </c>
@@ -2139,8 +2178,11 @@
       <c r="AC8" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>70</v>
       </c>
@@ -2177,8 +2219,11 @@
         <v>2</v>
       </c>
       <c r="S9" s="5"/>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AF9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>70</v>
       </c>
@@ -2206,8 +2251,14 @@
         <v>2</v>
       </c>
       <c r="S10" s="5"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE10" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>69</v>
       </c>
@@ -2250,7 +2301,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>71</v>
       </c>
@@ -2281,7 +2332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>71</v>
       </c>
@@ -2335,8 +2386,11 @@
       <c r="AC13" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AF13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>72</v>
       </c>
@@ -2376,8 +2430,11 @@
       <c r="AC14" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>73</v>
       </c>
@@ -2408,7 +2465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>73</v>
       </c>
@@ -2463,7 +2520,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>74</v>
       </c>
@@ -2504,7 +2561,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>75</v>
       </c>
@@ -2534,8 +2591,11 @@
       <c r="S18" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AF18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>75</v>
       </c>
@@ -2592,7 +2652,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>85</v>
       </c>
@@ -2646,8 +2706,11 @@
       <c r="AC20" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="23"/>
       <c r="B21" t="s">
         <v>92</v>
@@ -2678,7 +2741,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="23"/>
       <c r="B22" t="s">
         <v>91</v>
@@ -2730,8 +2793,11 @@
       <c r="AC22" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AF22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" t="s">
         <v>25</v>

</xml_diff>